<commit_message>
Updating excel file and script
</commit_message>
<xml_diff>
--- a/Fuzzing_rationale.xlsx
+++ b/Fuzzing_rationale.xlsx
@@ -1,21 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristanbrigham/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tristanbrigham/GithubProjects/NYUInternship/pop-paths-scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190C6AB1-FA5C-764F-8639-C46B6FC2DD77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CDDE6D0-9A75-A74E-9A7D-4AA09A90DFE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7440" yWindow="500" windowWidth="21360" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1884,7 +1896,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1965,8 +1977,33 @@
       <color theme="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2009,6 +2046,18 @@
         <bgColor rgb="FFC9DAF8"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor rgb="FFB7E1CD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2023,7 +2072,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -2057,6 +2106,16 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2287,8 +2346,8 @@
   </sheetPr>
   <dimension ref="A1:AO52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="94" workbookViewId="0">
-      <selection activeCell="J56" sqref="J56"/>
+    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2362,7 +2421,7 @@
       <c r="AO1" s="3"/>
     </row>
     <row r="2" spans="1:41" ht="41" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="4">
+      <c r="A2" s="21">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -2383,7 +2442,7 @@
       <c r="G2" s="5">
         <v>18</v>
       </c>
-      <c r="H2" s="7"/>
+      <c r="H2" s="22"/>
       <c r="I2" s="7" t="s">
         <v>153</v>
       </c>
@@ -2444,7 +2503,7 @@
       <c r="G3" s="5">
         <v>45</v>
       </c>
-      <c r="H3" s="7"/>
+      <c r="H3" s="22"/>
       <c r="I3" s="18" t="s">
         <v>11</v>
       </c>
@@ -2474,7 +2533,7 @@
       <c r="G4" s="5">
         <v>29</v>
       </c>
-      <c r="H4" s="7"/>
+      <c r="H4" s="22"/>
       <c r="I4" s="8" t="s">
         <v>13</v>
       </c>
@@ -2504,7 +2563,7 @@
       <c r="G5" s="5">
         <v>75</v>
       </c>
-      <c r="H5" s="7"/>
+      <c r="H5" s="22"/>
       <c r="I5" s="8" t="s">
         <v>16</v>
       </c>
@@ -2516,7 +2575,7 @@
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="23" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="6">
@@ -2534,7 +2593,7 @@
       <c r="G6" s="5">
         <v>64</v>
       </c>
-      <c r="H6" s="7"/>
+      <c r="H6" s="22"/>
       <c r="I6" s="8" t="s">
         <v>19</v>
       </c>
@@ -2563,7 +2622,7 @@
       <c r="G7" s="5">
         <v>43</v>
       </c>
-      <c r="H7" s="7"/>
+      <c r="H7" s="22"/>
       <c r="I7" s="8" t="s">
         <v>21</v>
       </c>
@@ -2593,7 +2652,7 @@
       <c r="G8" s="5">
         <v>48</v>
       </c>
-      <c r="H8" s="7"/>
+      <c r="H8" s="22"/>
       <c r="I8" s="10" t="s">
         <v>24</v>
       </c>
@@ -2605,7 +2664,7 @@
       <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="23" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="6">
@@ -2623,7 +2682,7 @@
       <c r="G9" s="5">
         <v>42</v>
       </c>
-      <c r="H9" s="7"/>
+      <c r="H9" s="22"/>
       <c r="I9" s="8" t="s">
         <v>27</v>
       </c>
@@ -2653,7 +2712,7 @@
       <c r="G10" s="5">
         <v>43</v>
       </c>
-      <c r="H10" s="7"/>
+      <c r="H10" s="22"/>
       <c r="I10" s="8" t="s">
         <v>30</v>
       </c>
@@ -2683,7 +2742,7 @@
       <c r="G11" s="5">
         <v>46</v>
       </c>
-      <c r="H11" s="7"/>
+      <c r="H11" s="22"/>
       <c r="I11" s="8" t="s">
         <v>32</v>
       </c>
@@ -2713,7 +2772,7 @@
       <c r="G12" s="5">
         <v>27</v>
       </c>
-      <c r="H12" s="7"/>
+      <c r="H12" s="22"/>
       <c r="I12" s="8" t="s">
         <v>35</v>
       </c>
@@ -2725,7 +2784,7 @@
       <c r="A13" s="4">
         <v>12</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="23" t="s">
         <v>37</v>
       </c>
       <c r="C13" s="6">
@@ -2743,7 +2802,7 @@
       <c r="G13" s="5">
         <v>22</v>
       </c>
-      <c r="H13" s="7"/>
+      <c r="H13" s="22"/>
       <c r="I13" s="10" t="s">
         <v>38</v>
       </c>
@@ -2753,7 +2812,7 @@
       <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="23" t="s">
         <v>39</v>
       </c>
       <c r="C14" s="6">
@@ -2771,7 +2830,7 @@
       <c r="G14" s="5">
         <v>56</v>
       </c>
-      <c r="H14" s="7"/>
+      <c r="H14" s="22"/>
       <c r="I14" s="8" t="s">
         <v>40</v>
       </c>
@@ -2801,7 +2860,7 @@
       <c r="G15" s="5">
         <v>63</v>
       </c>
-      <c r="H15" s="7"/>
+      <c r="H15" s="22"/>
       <c r="I15" s="8" t="s">
         <v>43</v>
       </c>
@@ -2829,7 +2888,7 @@
       <c r="G16" s="5">
         <v>40</v>
       </c>
-      <c r="H16" s="7"/>
+      <c r="H16" s="22"/>
       <c r="I16" s="8" t="s">
         <v>45</v>
       </c>
@@ -2841,7 +2900,7 @@
       <c r="A17" s="4">
         <v>16</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="23" t="s">
         <v>47</v>
       </c>
       <c r="C17" s="6">
@@ -2859,7 +2918,7 @@
       <c r="G17" s="5">
         <v>161791</v>
       </c>
-      <c r="H17" s="7"/>
+      <c r="H17" s="22"/>
       <c r="I17" s="8" t="s">
         <v>48</v>
       </c>
@@ -2871,7 +2930,7 @@
       <c r="A18" s="4">
         <v>17</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="23" t="s">
         <v>50</v>
       </c>
       <c r="C18" s="6">
@@ -2889,7 +2948,7 @@
       <c r="G18" s="5">
         <v>44</v>
       </c>
-      <c r="H18" s="7"/>
+      <c r="H18" s="22"/>
       <c r="I18" s="8" t="s">
         <v>51</v>
       </c>
@@ -2901,7 +2960,7 @@
       <c r="A19" s="4">
         <v>18</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="23" t="s">
         <v>53</v>
       </c>
       <c r="C19" s="6">
@@ -2919,7 +2978,7 @@
       <c r="G19" s="5">
         <v>27</v>
       </c>
-      <c r="H19" s="7"/>
+      <c r="H19" s="22"/>
       <c r="I19" s="8" t="s">
         <v>54</v>
       </c>
@@ -2931,7 +2990,7 @@
       <c r="A20" s="4">
         <v>19</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="23" t="s">
         <v>55</v>
       </c>
       <c r="C20" s="6">
@@ -2949,7 +3008,7 @@
       <c r="G20" s="5">
         <v>44</v>
       </c>
-      <c r="H20" s="7"/>
+      <c r="H20" s="22"/>
       <c r="I20" s="8" t="s">
         <v>56</v>
       </c>
@@ -2961,7 +3020,7 @@
       <c r="A21" s="4">
         <v>20</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="23" t="s">
         <v>57</v>
       </c>
       <c r="C21" s="6">
@@ -2979,7 +3038,7 @@
       <c r="G21" s="5">
         <v>69</v>
       </c>
-      <c r="H21" s="7"/>
+      <c r="H21" s="22"/>
       <c r="I21" s="7" t="s">
         <v>58</v>
       </c>
@@ -2991,7 +3050,7 @@
       <c r="A22" s="4">
         <v>21</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="23" t="s">
         <v>60</v>
       </c>
       <c r="C22" s="6">
@@ -3009,7 +3068,7 @@
       <c r="G22" s="5">
         <v>81</v>
       </c>
-      <c r="H22" s="7"/>
+      <c r="H22" s="22"/>
       <c r="I22" s="7" t="s">
         <v>61</v>
       </c>
@@ -3039,7 +3098,7 @@
       <c r="G23" s="5">
         <v>85</v>
       </c>
-      <c r="H23" s="7"/>
+      <c r="H23" s="22"/>
       <c r="I23" s="7" t="s">
         <v>64</v>
       </c>
@@ -3051,7 +3110,7 @@
       <c r="A24" s="4">
         <v>23</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="23" t="s">
         <v>66</v>
       </c>
       <c r="C24" s="6">
@@ -3069,7 +3128,7 @@
       <c r="G24" s="5">
         <v>114</v>
       </c>
-      <c r="H24" s="7"/>
+      <c r="H24" s="22"/>
       <c r="I24" s="8" t="s">
         <v>67</v>
       </c>
@@ -3099,7 +3158,7 @@
       <c r="G25" s="5">
         <v>83</v>
       </c>
-      <c r="H25" s="7"/>
+      <c r="H25" s="22"/>
       <c r="I25" s="8" t="s">
         <v>69</v>
       </c>
@@ -3129,7 +3188,7 @@
       <c r="G26" s="5">
         <v>84</v>
       </c>
-      <c r="H26" s="7"/>
+      <c r="H26" s="22"/>
       <c r="I26" s="7" t="s">
         <v>72</v>
       </c>
@@ -3141,7 +3200,7 @@
       <c r="A27" s="4">
         <v>26</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="23" t="s">
         <v>74</v>
       </c>
       <c r="C27" s="6">
@@ -3159,7 +3218,7 @@
       <c r="G27" s="5">
         <v>104</v>
       </c>
-      <c r="H27" s="7"/>
+      <c r="H27" s="22"/>
       <c r="I27" s="7" t="s">
         <v>75</v>
       </c>
@@ -3189,7 +3248,7 @@
       <c r="G28" s="5">
         <v>83</v>
       </c>
-      <c r="H28" s="7"/>
+      <c r="H28" s="22"/>
       <c r="I28" s="8" t="s">
         <v>78</v>
       </c>
@@ -3220,7 +3279,7 @@
       <c r="G29" s="5">
         <v>74</v>
       </c>
-      <c r="H29" s="7"/>
+      <c r="H29" s="22"/>
       <c r="I29" s="8" t="s">
         <v>81</v>
       </c>
@@ -3233,7 +3292,7 @@
       <c r="A30" s="4">
         <v>29</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="23" t="s">
         <v>83</v>
       </c>
       <c r="C30" s="6">
@@ -3251,7 +3310,7 @@
       <c r="G30" s="5">
         <v>27</v>
       </c>
-      <c r="H30" s="7"/>
+      <c r="H30" s="22"/>
       <c r="I30" s="7" t="s">
         <v>84</v>
       </c>
@@ -3281,7 +3340,7 @@
       <c r="G31" s="5">
         <v>376</v>
       </c>
-      <c r="H31" s="7"/>
+      <c r="H31" s="22"/>
       <c r="I31" s="8" t="s">
         <v>87</v>
       </c>
@@ -3311,7 +3370,7 @@
       <c r="G32" s="5">
         <v>47</v>
       </c>
-      <c r="H32" s="7"/>
+      <c r="H32" s="22"/>
       <c r="I32" s="7" t="s">
         <v>90</v>
       </c>
@@ -3371,7 +3430,7 @@
       <c r="G34" s="5">
         <v>84</v>
       </c>
-      <c r="H34" s="7"/>
+      <c r="H34" s="22"/>
       <c r="I34" s="7" t="s">
         <v>96</v>
       </c>
@@ -3383,7 +3442,7 @@
       <c r="A35" s="4">
         <v>34</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="23" t="s">
         <v>98</v>
       </c>
       <c r="C35" s="6">
@@ -3401,7 +3460,7 @@
       <c r="G35" s="5">
         <v>89</v>
       </c>
-      <c r="H35" s="7"/>
+      <c r="H35" s="22"/>
       <c r="I35" s="8" t="s">
         <v>99</v>
       </c>
@@ -3413,7 +3472,7 @@
       <c r="A36" s="4">
         <v>35</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="23" t="s">
         <v>101</v>
       </c>
       <c r="C36" s="6">
@@ -3431,7 +3490,7 @@
       <c r="G36" s="5">
         <v>178770</v>
       </c>
-      <c r="H36" s="7"/>
+      <c r="H36" s="22"/>
       <c r="I36" s="8" t="s">
         <v>102</v>
       </c>
@@ -3464,7 +3523,7 @@
       <c r="G37" s="5">
         <v>36</v>
       </c>
-      <c r="H37" s="7"/>
+      <c r="H37" s="22"/>
       <c r="I37" s="7" t="s">
         <v>106</v>
       </c>
@@ -3479,7 +3538,7 @@
       <c r="A38" s="4">
         <v>37</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="23" t="s">
         <v>109</v>
       </c>
       <c r="C38" s="6">
@@ -3497,7 +3556,7 @@
       <c r="G38" s="5">
         <v>84</v>
       </c>
-      <c r="H38" s="7"/>
+      <c r="H38" s="22"/>
       <c r="I38" s="7" t="s">
         <v>110</v>
       </c>
@@ -3512,7 +3571,7 @@
       <c r="A39" s="4">
         <v>38</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="23" t="s">
         <v>113</v>
       </c>
       <c r="C39" s="6">
@@ -3530,7 +3589,7 @@
       <c r="G39" s="5">
         <v>10</v>
       </c>
-      <c r="H39" s="7"/>
+      <c r="H39" s="22"/>
       <c r="I39" s="7" t="s">
         <v>114</v>
       </c>
@@ -3542,7 +3601,7 @@
       <c r="A40" s="4">
         <v>39</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="23" t="s">
         <v>116</v>
       </c>
       <c r="C40" s="6">
@@ -3560,7 +3619,7 @@
       <c r="G40" s="5">
         <v>199091</v>
       </c>
-      <c r="H40" s="7"/>
+      <c r="H40" s="22"/>
       <c r="I40" s="12" t="s">
         <v>117</v>
       </c>
@@ -3572,7 +3631,7 @@
       <c r="A41" s="4">
         <v>40</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="23" t="s">
         <v>119</v>
       </c>
       <c r="C41" s="6">
@@ -3590,7 +3649,7 @@
       <c r="G41" s="5">
         <v>466</v>
       </c>
-      <c r="H41" s="7"/>
+      <c r="H41" s="22"/>
       <c r="I41" s="8" t="s">
         <v>120</v>
       </c>
@@ -3602,7 +3661,7 @@
       <c r="A42" s="4">
         <v>41</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="23" t="s">
         <v>121</v>
       </c>
       <c r="C42" s="6">
@@ -3620,7 +3679,7 @@
       <c r="G42" s="5">
         <v>164484</v>
       </c>
-      <c r="H42" s="7"/>
+      <c r="H42" s="22"/>
       <c r="I42" s="8" t="s">
         <v>122</v>
       </c>
@@ -3650,7 +3709,7 @@
       <c r="G43" s="5">
         <v>79</v>
       </c>
-      <c r="H43" s="7"/>
+      <c r="H43" s="22"/>
       <c r="I43" s="8" t="s">
         <v>125</v>
       </c>
@@ -3662,7 +3721,7 @@
       <c r="A44" s="4">
         <v>43</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="23" t="s">
         <v>127</v>
       </c>
       <c r="C44" s="6">
@@ -3680,7 +3739,7 @@
       <c r="G44" s="5">
         <v>71</v>
       </c>
-      <c r="H44" s="7"/>
+      <c r="H44" s="22"/>
       <c r="I44" s="7" t="s">
         <v>128</v>
       </c>
@@ -3692,7 +3751,7 @@
       <c r="A45" s="4">
         <v>44</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="23" t="s">
         <v>130</v>
       </c>
       <c r="C45" s="6">
@@ -3710,7 +3769,7 @@
       <c r="G45" s="5">
         <v>58</v>
       </c>
-      <c r="H45" s="7"/>
+      <c r="H45" s="22"/>
       <c r="I45" s="8" t="s">
         <v>131</v>
       </c>
@@ -3743,7 +3802,7 @@
       <c r="G46" s="5">
         <v>41</v>
       </c>
-      <c r="H46" s="7"/>
+      <c r="H46" s="22"/>
       <c r="I46" s="8" t="s">
         <v>135</v>
       </c>
@@ -3773,8 +3832,8 @@
       <c r="G47" s="5">
         <v>18849</v>
       </c>
-      <c r="H47" s="7"/>
-      <c r="I47" s="8" t="s">
+      <c r="H47" s="26"/>
+      <c r="I47" s="24" t="s">
         <v>138</v>
       </c>
       <c r="J47" s="8" t="s">
@@ -3785,7 +3844,7 @@
       <c r="A48" s="4">
         <v>47</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="23" t="s">
         <v>140</v>
       </c>
       <c r="C48" s="6">
@@ -3803,7 +3862,7 @@
       <c r="G48" s="5">
         <v>62</v>
       </c>
-      <c r="H48" s="7"/>
+      <c r="H48" s="22"/>
       <c r="I48" s="8" t="s">
         <v>141</v>
       </c>
@@ -3834,7 +3893,7 @@
       <c r="G49" s="5">
         <v>72</v>
       </c>
-      <c r="H49" s="7"/>
+      <c r="H49" s="22"/>
       <c r="I49" s="7" t="s">
         <v>144</v>
       </c>
@@ -3866,7 +3925,7 @@
         <v>272</v>
       </c>
       <c r="H50" s="7"/>
-      <c r="I50" s="7" t="s">
+      <c r="I50" s="25" t="s">
         <v>147</v>
       </c>
       <c r="J50" s="14" t="s">
@@ -3878,7 +3937,7 @@
       <c r="A51" s="4">
         <v>50</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B51" s="23" t="s">
         <v>149</v>
       </c>
       <c r="C51" s="6">

</xml_diff>